<commit_message>
remove ancilliary confirmed and actual load, change number format form 2 decimals to 4 decimals
</commit_message>
<xml_diff>
--- a/Immediate Viewer.xlsx
+++ b/Immediate Viewer.xlsx
@@ -15,15 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
-    <t>Date: 2021-07-06</t>
+    <t>Date: 2021-07-12</t>
   </si>
   <si>
     <t xml:space="preserve">Unit: </t>
-  </si>
-  <si>
-    <t>ANCILLARY OFFERED</t>
   </si>
   <si>
     <t>ANCILLARY CONFIRMED</t>
@@ -36,9 +33,6 @@
   </si>
   <si>
     <t>Capacity</t>
-  </si>
-  <si>
-    <t>Actual Load</t>
   </si>
   <si>
     <t>Metered Q</t>
@@ -76,21 +70,21 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial Black"/>
     </font>
     <font>
       <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial Black"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,12 +97,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDFFAAA"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF83F997"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -139,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -152,26 +140,32 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,51 +498,43 @@
       <c r="O1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8"/>
       <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
       <c r="O2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="3">
@@ -566,16 +552,14 @@
       <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
       <c r="I3" s="2">
         <v>0</v>
       </c>
-      <c r="J3" s="2">
-        <v>8042.348333</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="4">
         <v>0</v>
       </c>
@@ -584,11 +568,9 @@
       <c r="O3" s="5">
         <v>0</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="3">
@@ -606,16 +588,14 @@
       <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
-      <c r="J4" s="2">
-        <v>2622.680833</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="4">
         <v>0</v>
       </c>
@@ -624,11 +604,9 @@
       <c r="O4" s="5">
         <v>0</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="3">
@@ -646,16 +624,14 @@
       <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
-      <c r="J5" s="2">
-        <v>2360.320833</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="4">
         <v>0</v>
       </c>
@@ -664,11 +640,9 @@
       <c r="O5" s="5">
         <v>0</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5">
-        <v>0</v>
-      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="3">
@@ -686,16 +660,14 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
       <c r="I6" s="2">
         <v>0</v>
       </c>
-      <c r="J6" s="2">
-        <v>2243.01</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="4">
         <v>0</v>
       </c>
@@ -704,11 +676,9 @@
       <c r="O6" s="5">
         <v>0</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5">
-        <v>0</v>
-      </c>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="3">
@@ -726,16 +696,14 @@
       <c r="G7" s="2">
         <v>0</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
       <c r="I7" s="2">
         <v>0</v>
       </c>
-      <c r="J7" s="2">
-        <v>2309.663333</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="4">
         <v>0</v>
       </c>
@@ -744,11 +712,9 @@
       <c r="O7" s="5">
         <v>0</v>
       </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5">
-        <v>0</v>
-      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="3">
@@ -766,16 +732,14 @@
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
       <c r="I8" s="2">
         <v>0</v>
       </c>
-      <c r="J8" s="2">
-        <v>2413.688333</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="4">
         <v>0</v>
       </c>
@@ -784,11 +748,9 @@
       <c r="O8" s="5">
         <v>0</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5">
-        <v>0</v>
-      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="3">
@@ -806,16 +768,14 @@
       <c r="G9" s="2">
         <v>0</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
       <c r="I9" s="2">
         <v>0</v>
       </c>
-      <c r="J9" s="2">
-        <v>1675.878333</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="4">
         <v>0</v>
       </c>
@@ -824,11 +784,9 @@
       <c r="O9" s="5">
         <v>0</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5">
-        <v>0</v>
-      </c>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="3">
@@ -846,16 +804,14 @@
       <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
       <c r="I10" s="2">
         <v>0</v>
       </c>
-      <c r="J10" s="2">
-        <v>1958.075833</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="4">
         <v>0</v>
       </c>
@@ -864,11 +820,9 @@
       <c r="O10" s="5">
         <v>0</v>
       </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5">
-        <v>0</v>
-      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="3">
@@ -886,16 +840,14 @@
       <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
       <c r="I11" s="2">
         <v>0</v>
       </c>
-      <c r="J11" s="2">
-        <v>8995.636667</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="4">
         <v>0</v>
       </c>
@@ -904,11 +856,9 @@
       <c r="O11" s="5">
         <v>0</v>
       </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5">
-        <v>0</v>
-      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="3">
@@ -926,16 +876,14 @@
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
       <c r="I12" s="2">
         <v>0</v>
       </c>
-      <c r="J12" s="2">
-        <v>5532.525</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="4">
         <v>0</v>
       </c>
@@ -944,11 +892,9 @@
       <c r="O12" s="5">
         <v>0</v>
       </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5">
-        <v>0</v>
-      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="3">
@@ -966,16 +912,14 @@
       <c r="G13" s="2">
         <v>0</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
       <c r="I13" s="2">
         <v>0</v>
       </c>
-      <c r="J13" s="2">
-        <v>10841.745833</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="4">
         <v>0</v>
       </c>
@@ -984,11 +928,9 @@
       <c r="O13" s="5">
         <v>0</v>
       </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5">
-        <v>0</v>
-      </c>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="3">
@@ -1006,16 +948,14 @@
       <c r="G14" s="2">
         <v>0</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="J14" s="2">
-        <v>7741.599167</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="4">
         <v>0</v>
       </c>
@@ -1024,11 +964,9 @@
       <c r="O14" s="5">
         <v>0</v>
       </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5">
-        <v>0</v>
-      </c>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="3">
@@ -1046,16 +984,14 @@
       <c r="G15" s="2">
         <v>0</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
       <c r="I15" s="2">
         <v>0</v>
       </c>
-      <c r="J15" s="2">
-        <v>5070.478333</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="4">
         <v>0</v>
       </c>
@@ -1064,11 +1000,9 @@
       <c r="O15" s="5">
         <v>0</v>
       </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5">
-        <v>0</v>
-      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="3">
@@ -1086,16 +1020,14 @@
       <c r="G16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="J16" s="2">
-        <v>7203.69</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0</v>
-      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="4">
         <v>0</v>
       </c>
@@ -1104,11 +1036,9 @@
       <c r="O16" s="5">
         <v>0</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5">
-        <v>0</v>
-      </c>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="3">
@@ -1126,16 +1056,14 @@
       <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="J17" s="2">
-        <v>11137.143333</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="4">
         <v>0</v>
       </c>
@@ -1144,11 +1072,9 @@
       <c r="O17" s="5">
         <v>0</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5">
-        <v>0</v>
-      </c>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="3">
@@ -1166,16 +1092,14 @@
       <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
       <c r="I18" s="2">
         <v>0</v>
       </c>
-      <c r="J18" s="2">
-        <v>4763.305</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0</v>
-      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="4">
         <v>0</v>
       </c>
@@ -1184,11 +1108,9 @@
       <c r="O18" s="5">
         <v>0</v>
       </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5">
-        <v>0</v>
-      </c>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="3">
@@ -1206,16 +1128,14 @@
       <c r="G19" s="2">
         <v>0</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
       <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="J19" s="2">
-        <v>3616.216667</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="4">
         <v>0</v>
       </c>
@@ -1224,11 +1144,9 @@
       <c r="O19" s="5">
         <v>0</v>
       </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5">
-        <v>0</v>
-      </c>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="3">
@@ -1246,16 +1164,14 @@
       <c r="G20" s="2">
         <v>0</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="J20" s="2">
-        <v>2952.0125</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0</v>
-      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="4">
         <v>0</v>
       </c>
@@ -1264,11 +1180,9 @@
       <c r="O20" s="5">
         <v>0</v>
       </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5">
-        <v>0</v>
-      </c>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="3">
@@ -1286,16 +1200,14 @@
       <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
       <c r="I21" s="2">
         <v>0</v>
       </c>
-      <c r="J21" s="2">
-        <v>10941.914167</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0</v>
-      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
       <c r="L21" s="4">
         <v>0</v>
       </c>
@@ -1304,11 +1216,9 @@
       <c r="O21" s="5">
         <v>0</v>
       </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5">
-        <v>0</v>
-      </c>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="3">
@@ -1326,16 +1236,14 @@
       <c r="G22" s="2">
         <v>0</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="J22" s="2">
-        <v>2903.705833</v>
-      </c>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
       <c r="L22" s="4">
         <v>0</v>
       </c>
@@ -1344,11 +1252,9 @@
       <c r="O22" s="5">
         <v>0</v>
       </c>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5">
-        <v>0</v>
-      </c>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="3">
@@ -1366,16 +1272,14 @@
       <c r="G23" s="2">
         <v>0</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="J23" s="2">
-        <v>5801.240833</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
       <c r="L23" s="4">
         <v>0</v>
       </c>
@@ -1384,11 +1288,9 @@
       <c r="O23" s="5">
         <v>0</v>
       </c>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5">
-        <v>0</v>
-      </c>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="3">
@@ -1406,16 +1308,14 @@
       <c r="G24" s="2">
         <v>0</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
       <c r="I24" s="2">
         <v>0</v>
       </c>
-      <c r="J24" s="2">
-        <v>3574.6525</v>
-      </c>
-      <c r="K24" s="2">
-        <v>0</v>
-      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="4">
         <v>0</v>
       </c>
@@ -1424,11 +1324,9 @@
       <c r="O24" s="5">
         <v>0</v>
       </c>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5">
-        <v>0</v>
-      </c>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="3">
@@ -1446,16 +1344,14 @@
       <c r="G25" s="2">
         <v>0</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
       <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <v>0</v>
-      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="4">
         <v>0</v>
       </c>
@@ -1464,11 +1360,9 @@
       <c r="O25" s="5">
         <v>0</v>
       </c>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5">
-        <v>0</v>
-      </c>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="3">
@@ -1486,16 +1380,14 @@
       <c r="G26" s="2">
         <v>0</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
       <c r="I26" s="2">
         <v>0</v>
       </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
       <c r="L26" s="4">
         <v>0</v>
       </c>
@@ -1504,11 +1396,9 @@
       <c r="O26" s="5">
         <v>0</v>
       </c>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5">
-        <v>0</v>
-      </c>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1516,157 +1406,106 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
     <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:Q7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
     <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
     <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O12:Q12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
     <mergeCell ref="L13:N13"/>
-    <mergeCell ref="O13:Q13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
     <mergeCell ref="L14:N14"/>
-    <mergeCell ref="O14:Q14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O15:Q15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="L16:N16"/>
-    <mergeCell ref="O16:Q16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="L17:N17"/>
-    <mergeCell ref="O17:Q17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:Q18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:Q19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="L20:N20"/>
-    <mergeCell ref="O20:Q20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
     <mergeCell ref="L21:N21"/>
-    <mergeCell ref="O21:Q21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="L22:N22"/>
-    <mergeCell ref="O22:Q22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
     <mergeCell ref="L23:N23"/>
-    <mergeCell ref="O23:Q23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
     <mergeCell ref="L24:N24"/>
-    <mergeCell ref="O24:Q24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
     <mergeCell ref="L25:N25"/>
-    <mergeCell ref="O25:Q25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
     <mergeCell ref="L26:N26"/>
-    <mergeCell ref="O26:Q26"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
     <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:Q1"/>
     <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>